<commit_message>
- fix lỗi xuất file DS KhachHang: không hiện dòngTổng cộng
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhSachKhachHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>DANH SÁCH KHÁCH HÀNG</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Số tài khoản</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +154,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -175,12 +184,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,34 +323,37 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -621,11 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,32 +689,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
       <c r="Y1" s="6"/>
     </row>
     <row r="3" spans="1:25" s="13" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1351,73 +1389,102 @@
       <c r="W26" s="26"/>
       <c r="X26" s="26"/>
     </row>
-    <row r="27" spans="1:24" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="37"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="39">
-        <f>SUM(R4:R26)</f>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="26"/>
+    </row>
+    <row r="28" spans="1:24" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="40">
+        <f>SUM(R$4:R26)</f>
         <v>0</v>
       </c>
-      <c r="S27" s="39">
-        <f>SUM(S4:S26)</f>
+      <c r="S28" s="40">
+        <f>SUM(S$4:S26)</f>
         <v>0</v>
       </c>
-      <c r="T27" s="39">
-        <f>SUM(T4:T26)</f>
+      <c r="T28" s="40">
+        <f>SUM(T$4:T26)</f>
         <v>0</v>
       </c>
-      <c r="U27" s="39">
-        <f>SUM(U4:U26)</f>
+      <c r="U28" s="40">
+        <f>SUM(U$4:U26)</f>
         <v>0</v>
       </c>
-      <c r="V27" s="42"/>
-      <c r="W27" s="44"/>
-      <c r="X27" s="44"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
+      <c r="V28" s="43"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>